<commit_message>
Validation on first_name, bulk ingest
</commit_message>
<xml_diff>
--- a/api/order/sample_sheets/current.xlsx
+++ b/api/order/sample_sheets/current.xlsx
@@ -16,6 +16,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">Sheet1!$11:$11</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0" vbProcedure="false">Sheet1!$11:$11</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0" vbProcedure="false">Sheet1!$11:$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0" vbProcedure="false">Sheet1!$11:$11</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -1195,9 +1196,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2294640</xdr:colOff>
+      <xdr:colOff>2294280</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>104040</xdr:rowOff>
+      <xdr:rowOff>103680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1207,7 +1208,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6660720" y="9360"/>
-          <a:ext cx="817920" cy="594720"/>
+          <a:ext cx="817560" cy="594360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1235,9 +1236,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2694600</xdr:colOff>
+      <xdr:colOff>2694240</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>332640</xdr:rowOff>
+      <xdr:rowOff>332280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1251,7 +1252,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1390680" y="66600"/>
-          <a:ext cx="1303920" cy="766080"/>
+          <a:ext cx="1303560" cy="765720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1276,7 +1277,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topRight" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1486,7 +1487,9 @@
       <c r="B18" s="29" t="n">
         <v>1</v>
       </c>
-      <c r="C18" s="31"/>
+      <c r="C18" s="31" t="n">
+        <v>1</v>
+      </c>
       <c r="D18" s="30" t="n">
         <v>1.35</v>
       </c>

</xml_diff>

<commit_message>
Bug fix: Unique filename on upload to processed dropbox folder
</commit_message>
<xml_diff>
--- a/api/order/sample_sheets/current.xlsx
+++ b/api/order/sample_sheets/current.xlsx
@@ -17,6 +17,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0" vbProcedure="false">Sheet1!$11:$11</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0" vbProcedure="false">Sheet1!$11:$11</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0" vbProcedure="false">Sheet1!$11:$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0" vbProcedure="false">Sheet1!$11:$11</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -1196,9 +1197,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2294280</xdr:colOff>
+      <xdr:colOff>2293920</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>103680</xdr:rowOff>
+      <xdr:rowOff>103320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1208,7 +1209,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6660720" y="9360"/>
-          <a:ext cx="817560" cy="594360"/>
+          <a:ext cx="817200" cy="594000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1236,9 +1237,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2694240</xdr:colOff>
+      <xdr:colOff>2693880</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>332280</xdr:rowOff>
+      <xdr:rowOff>331920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1252,7 +1253,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1390680" y="66600"/>
-          <a:ext cx="1303560" cy="765720"/>
+          <a:ext cx="1303200" cy="765360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1277,7 +1278,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="topRight" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2804,7 +2805,7 @@
   <dimension ref="A1:A72"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="1" sqref="C4 D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>